<commit_message>
component approach to pulling URLs and data-anas
</commit_message>
<xml_diff>
--- a/validation_sheet.xlsx
+++ b/validation_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irraghavdev/repos/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavsharma/repos/personal-gh/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F5DE7C-413E-6A4A-A47C-CF8A13DB69A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFAB847-EA0B-934C-B38C-63C9B387626F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{FE62ADD2-636B-2B46-8FD0-709D22FD913D}"/>
+    <workbookView xWindow="3820" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{FE62ADD2-636B-2B46-8FD0-709D22FD913D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Attributes Pages" sheetId="2" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>URL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>https://www.bmo.com/main/personal</t>
   </si>
@@ -397,36 +394,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7533D9-C72E-C748-B895-F41F185D1698}">
-  <dimension ref="C2:C4"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{5D458F50-B84C-1D4A-B31A-5C3426CAA293}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{EA6CFE22-CE13-534F-8EC7-56311D5E7A59}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5D458F50-B84C-1D4A-B31A-5C3426CAA293}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{EA6CFE22-CE13-534F-8EC7-56311D5E7A59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>